<commit_message>
Latest changes to framework.
</commit_message>
<xml_diff>
--- a/model_constraints/trn_constraints_ref.xlsx
+++ b/model_constraints/trn_constraints_ref.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/rashid_zetter_mail_utoronto_ca/Documents/Documents/Research/CANOE-transportation/model_constraints/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1570" documentId="8_{D5DFC8B2-0017-4459-95F4-B0338769A746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC714CF1-B07A-462A-B7AB-910530A7D930}"/>
+  <xr:revisionPtr revIDLastSave="1573" documentId="8_{D5DFC8B2-0017-4459-95F4-B0338769A746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A91ABF42-8420-44AB-8B4B-A8888EBBD7DA}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" firstSheet="4" activeTab="8" xr2:uid="{B100FC8B-7A95-4426-88DD-41697D720D42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{B100FC8B-7A95-4426-88DD-41697D720D42}"/>
   </bookViews>
   <sheets>
     <sheet name="CostEmission" sheetId="1" r:id="rId1"/>
@@ -900,15 +900,15 @@
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6328125" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" customWidth="1"/>
-    <col min="6" max="6" width="101.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="101.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +931,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -954,7 +954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -977,7 +977,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1023,7 +1023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1105,12 +1105,12 @@
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1297,7 +1297,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1518,7 +1518,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>7</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1552,7 +1552,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1569,7 +1569,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>7</v>
       </c>
@@ -1637,7 +1637,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>7</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="37" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
@@ -1739,7 +1739,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -1790,7 +1790,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>7</v>
       </c>
@@ -1824,7 +1824,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -1858,7 +1858,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>7</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1943,7 +1943,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>7</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -2211,12 +2211,12 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2224,142 +2224,142 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>117</v>
       </c>
@@ -2377,13 +2377,13 @@
       <selection activeCell="B77" activeCellId="2" sqref="B65 B71 B77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.90625" customWidth="1"/>
-    <col min="2" max="2" width="23.90625" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2399,7 +2399,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2439,7 +2439,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2487,7 +2487,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2511,7 +2511,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -2519,7 +2519,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -2527,7 +2527,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -2535,7 +2535,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="23" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="24" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="31" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -2631,7 +2631,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>29</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>30</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -2679,7 +2679,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -2687,7 +2687,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -2727,7 +2727,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -2767,7 +2767,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>44</v>
       </c>
@@ -2783,7 +2783,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="51" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -2791,7 +2791,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>46</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>47</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="54" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>48</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>49</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>50</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>51</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="58" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>52</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="59" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>53</v>
       </c>
@@ -2855,7 +2855,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>54</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="61" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>56</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>57</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="64" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>58</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>22</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>23</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>12</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>13</v>
       </c>
@@ -2927,7 +2927,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>14</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>28</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>29</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>30</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>31</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>32</v>
       </c>
@@ -2983,7 +2983,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>33</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>40</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>41</v>
       </c>
@@ -3015,7 +3015,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>42</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>43</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>44</v>
       </c>
@@ -3039,7 +3039,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>18</v>
       </c>
@@ -3047,7 +3047,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -3055,7 +3055,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>20</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>21</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>22</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>23</v>
       </c>
@@ -3087,7 +3087,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>12</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>13</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>14</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>24</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>25</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>26</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>27</v>
       </c>
@@ -3159,7 +3159,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>28</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>29</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>30</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>31</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>32</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>33</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>34</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>35</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>36</v>
       </c>
@@ -3231,7 +3231,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>37</v>
       </c>
@@ -3239,7 +3239,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>38</v>
       </c>
@@ -3247,7 +3247,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>39</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>40</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>41</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>42</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>43</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>44</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>45</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>46</v>
       </c>
@@ -3311,7 +3311,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>47</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>48</v>
       </c>
@@ -3327,7 +3327,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>49</v>
       </c>
@@ -3335,7 +3335,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>50</v>
       </c>
@@ -3343,7 +3343,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>51</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>52</v>
       </c>
@@ -3359,7 +3359,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>53</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>54</v>
       </c>
@@ -3375,7 +3375,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>55</v>
       </c>
@@ -3383,7 +3383,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>56</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>57</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="128" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>58</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>18</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>19</v>
       </c>
@@ -3423,7 +3423,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>20</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>21</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>22</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>23</v>
       </c>
@@ -3455,7 +3455,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>12</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>13</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>14</v>
       </c>
@@ -3479,7 +3479,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>15</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>16</v>
       </c>
@@ -3495,7 +3495,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>24</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>25</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>26</v>
       </c>
@@ -3519,7 +3519,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>27</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>28</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>29</v>
       </c>
@@ -3543,7 +3543,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>30</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>31</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>32</v>
       </c>
@@ -3567,7 +3567,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>33</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>34</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>35</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>36</v>
       </c>
@@ -3599,7 +3599,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>37</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>38</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>39</v>
       </c>
@@ -3623,7 +3623,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>40</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>41</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>42</v>
       </c>
@@ -3647,7 +3647,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>43</v>
       </c>
@@ -3655,7 +3655,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>44</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>45</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>46</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>47</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>48</v>
       </c>
@@ -3695,7 +3695,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>49</v>
       </c>
@@ -3703,7 +3703,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>50</v>
       </c>
@@ -3711,7 +3711,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>51</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>52</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>53</v>
       </c>
@@ -3735,7 +3735,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>54</v>
       </c>
@@ -3743,7 +3743,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>55</v>
       </c>
@@ -3751,7 +3751,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>56</v>
       </c>
@@ -3759,7 +3759,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>57</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="174" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>58</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>107</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>108</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>109</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>104</v>
       </c>
@@ -3807,7 +3807,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>72</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>73</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>74</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>75</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>110</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>111</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>112</v>
       </c>
@@ -3863,7 +3863,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>105</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>76</v>
       </c>
@@ -3879,7 +3879,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>77</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>78</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>79</v>
       </c>
@@ -3903,7 +3903,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>113</v>
       </c>
@@ -3911,7 +3911,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>114</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>106</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>80</v>
       </c>
@@ -3935,7 +3935,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>81</v>
       </c>
@@ -3952,19 +3952,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D16FFEAC-7CBA-4133-9327-20E933AD6B31}">
   <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="66.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3984,7 +3984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -4004,7 +4004,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -4364,7 +4364,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -4404,7 +4404,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -4424,7 +4424,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -4441,7 +4441,7 @@
         <v>0.68479999999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>0.68020000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -4492,7 +4492,7 @@
         <v>0.72550000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -4509,7 +4509,7 @@
         <v>0.1195</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>0.34689999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -4560,7 +4560,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>0.10440000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>0.1011</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -4611,7 +4611,7 @@
         <v>4.6300000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>0.58209999999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>0.57820000000000005</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -4662,7 +4662,7 @@
         <v>2.8500000000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>0.65290000000000004</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>0.1076</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -4713,7 +4713,7 @@
         <v>0.31219999999999998</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -4730,7 +4730,7 @@
         <v>0.49769999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>7</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>0.90249999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>7</v>
       </c>
@@ -4764,7 +4764,7 @@
         <v>0.1148</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>0.11119999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>7</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>5.0900000000000001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>7</v>
       </c>
@@ -4815,7 +4815,7 @@
         <v>0.49480000000000002</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>7</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>0.4914</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>7</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -4866,7 +4866,7 @@
         <v>0.58760000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -4883,7 +4883,7 @@
         <v>9.6799999999999997E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>7</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>0.28100000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>7</v>
       </c>
@@ -4917,7 +4917,7 @@
         <v>0.44790000000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>7</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>0.85740000000000005</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>7</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>0.1263</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>7</v>
       </c>
@@ -4968,7 +4968,7 @@
         <v>0.12230000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -4985,7 +4985,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>7</v>
       </c>
@@ -5002,7 +5002,7 @@
         <v>0.42049999999999998</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>7</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>0.41770000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>7</v>
       </c>
@@ -5036,7 +5036,7 @@
         <v>2.06E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>7</v>
       </c>
@@ -5053,7 +5053,7 @@
         <v>0.52890000000000004</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>7</v>
       </c>
@@ -5070,7 +5070,7 @@
         <v>8.7099999999999997E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>7</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>0.25290000000000001</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>7</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>0.40310000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>7</v>
       </c>
@@ -5121,7 +5121,7 @@
         <v>0.8145</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>0.1389</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -5155,7 +5155,7 @@
         <v>0.13450000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>7</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>6.1600000000000002E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>0.35749999999999998</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>7</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>0.35510000000000003</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>7</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>7</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>0.47599999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>7</v>
       </c>
@@ -5257,7 +5257,7 @@
         <v>7.8399999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>7</v>
       </c>
@@ -5274,7 +5274,7 @@
         <v>0.2276</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>7</v>
       </c>
@@ -5291,7 +5291,7 @@
         <v>0.36280000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>7</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>0.77380000000000004</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>7</v>
       </c>
@@ -5325,7 +5325,7 @@
         <v>0.15279999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>7</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>0.14799999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>7</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>6.7799999999999999E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>7</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>0.30380000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>7</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>0.30180000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>7</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>1.49E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>7</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>0.4284</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>7</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>7.0599999999999996E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>7</v>
       </c>
@@ -5461,7 +5461,7 @@
         <v>0.20480000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>7</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>0.32650000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>7</v>
       </c>
@@ -5495,7 +5495,7 @@
         <v>0.73509999999999998</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>7</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>0.1681</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>7</v>
       </c>
@@ -5529,7 +5529,7 @@
         <v>0.1628</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>7</v>
       </c>
@@ -5559,14 +5559,14 @@
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5600,7 +5600,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5617,7 +5617,7 @@
         <v>2.2599999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>4.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -5668,7 +5668,7 @@
         <v>3.3500000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>2.07E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -5719,7 +5719,7 @@
         <v>4.7100000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -5736,7 +5736,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -5753,7 +5753,7 @@
         <v>2.86E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>6.2899999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -5787,7 +5787,7 @@
         <v>1.34E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -5804,7 +5804,7 @@
         <v>3.6600000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>7.9399999999999998E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>1.6899999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -5855,7 +5855,7 @@
         <v>4.3999999999999997E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -5872,7 +5872,7 @@
         <v>9.5299999999999996E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -5898,19 +5898,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D18C4C-06FD-4063-9CD7-88D489A10BB6}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" customWidth="1"/>
-    <col min="6" max="6" width="56.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="56.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -5950,7 +5950,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -5970,7 +5970,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -6010,7 +6010,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -6030,7 +6030,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -6050,7 +6050,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6070,7 +6070,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -6090,7 +6090,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -6110,7 +6110,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -6170,7 +6170,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -6210,7 +6210,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -6250,7 +6250,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -6270,7 +6270,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -6310,7 +6310,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -6350,7 +6350,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -6370,7 +6370,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -6410,7 +6410,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -6450,7 +6450,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -6470,7 +6470,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -6510,7 +6510,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -6530,7 +6530,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -6550,7 +6550,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -6570,7 +6570,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -6590,7 +6590,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -6610,7 +6610,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -6650,7 +6650,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -6690,7 +6690,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>7</v>
       </c>
@@ -6723,14 +6723,14 @@
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
-    <col min="5" max="5" width="127.90625" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="127.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6750,7 +6750,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -6770,7 +6770,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -6790,7 +6790,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -6810,7 +6810,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -6850,7 +6850,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -6870,7 +6870,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -6910,7 +6910,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -6930,7 +6930,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -6950,7 +6950,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -6990,7 +6990,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -7050,7 +7050,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -7070,7 +7070,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -7090,7 +7090,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -7130,7 +7130,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -7150,7 +7150,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -7190,7 +7190,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -7250,7 +7250,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -7270,7 +7270,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -7290,7 +7290,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -7370,7 +7370,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -7390,7 +7390,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -7410,7 +7410,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -7430,7 +7430,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -7450,7 +7450,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -7470,7 +7470,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -7490,7 +7490,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -7519,18 +7519,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE35148D-414B-46BB-8E73-1793A97E541C}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="12" customWidth="1"/>
-    <col min="9" max="9" width="42.81640625" customWidth="1"/>
+    <col min="9" max="9" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7562,7 +7562,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -7594,7 +7594,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -7658,7 +7658,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -7722,7 +7722,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -7818,7 +7818,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -7883,7 +7883,7 @@
       </c>
       <c r="L11"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -7915,7 +7915,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -7947,7 +7947,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -8011,7 +8011,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -8043,7 +8043,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -8107,7 +8107,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -8172,7 +8172,7 @@
       </c>
       <c r="L20"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -8204,7 +8204,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -8236,7 +8236,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -8300,7 +8300,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -8332,7 +8332,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -8396,7 +8396,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -8428,7 +8428,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>7</v>
       </c>
@@ -8461,7 +8461,7 @@
       </c>
       <c r="L29"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -8493,7 +8493,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -8525,7 +8525,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>7</v>
       </c>
@@ -8592,7 +8592,7 @@
       <c r="L33"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>7</v>
       </c>
@@ -8626,7 +8626,7 @@
       <c r="K34" s="2"/>
       <c r="M34" s="2"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -8658,7 +8658,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
@@ -8690,7 +8690,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>7</v>
       </c>
@@ -8722,7 +8722,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>7</v>
       </c>
@@ -8754,7 +8754,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>7</v>
       </c>

</xml_diff>